<commit_message>
fix: changes for product update
</commit_message>
<xml_diff>
--- a/Input/Product_Offer/ProductOfferOld.xlsx
+++ b/Input/Product_Offer/ProductOfferOld.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,63 +467,51 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>23070502</v>
+        <v>22101901</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Kwat Ti Po Ya 9999ks</t>
+          <t>Super 10K</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>23042501</v>
+        <v>22101902</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Kwat Ti Po Ya 1999ks</t>
+          <t>Super 15K</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>23052603</v>
+        <v>23031502</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Kwat Ti Po Ya 1996ks</t>
+          <t>Super 25K</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>21021903</v>
+        <v>23032502</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Talkie Suboo 999ks</t>
+          <t>Super 35K</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>23030305</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>On net 999ks</t>
-        </is>
-      </c>
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>20050522</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Data Suboo 949ks</t>
-        </is>
-      </c>
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>

</xml_diff>